<commit_message>
Adding the files with new data , commenting the code which writes into the file to avoid overriding the content into the files
</commit_message>
<xml_diff>
--- a/yt_multi_language_ui_validator/src/main/resources/data/verifyingGlobalFilterLandingPage.xlsx
+++ b/yt_multi_language_ui_validator/src/main/resources/data/verifyingGlobalFilterLandingPage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sagar\youtube-multi-language-ui-validator-automation\yt_multi_language_ui_validator\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498C32CB-21E6-4C08-B551-0668CF225800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB5F5CE-E6D9-43A9-9A9A-DB57F9CAFA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2002,10 +2002,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2329,431 +2329,431 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="138.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="53.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="139.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding column header names in the respective data sheets
</commit_message>
<xml_diff>
--- a/yt_multi_language_ui_validator/src/main/resources/data/verifyingGlobalFilterLandingPage.xlsx
+++ b/yt_multi_language_ui_validator/src/main/resources/data/verifyingGlobalFilterLandingPage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sagar\youtube-multi-language-ui-validator-automation\yt_multi_language_ui_validator\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB5F5CE-E6D9-43A9-9A9A-DB57F9CAFA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B004C2-AFA7-41F1-999A-B0D2CD3EC6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
   <si>
     <t>Afrikaans</t>
   </si>
@@ -1964,6 +1964,12 @@
 업로드 날짜
 조회수
 평점</t>
+  </si>
+  <si>
+    <t>Applied Language</t>
+  </si>
+  <si>
+    <t>Expected Data</t>
   </si>
 </sst>
 </file>
@@ -2321,10 +2327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B54"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2333,6 +2339,14 @@
     <col min="2" max="2" width="139.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Runnig the tests without headless
</commit_message>
<xml_diff>
--- a/yt_multi_language_ui_validator/src/main/resources/data/verifyingGlobalFilterLandingPage.xlsx
+++ b/yt_multi_language_ui_validator/src/main/resources/data/verifyingGlobalFilterLandingPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sagar\youtube-multi-language-ui-validator-automation\yt_multi_language_ui_validator\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B004C2-AFA7-41F1-999A-B0D2CD3EC6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A2BA3F-BBB3-4005-876A-1724294BF448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verifyingGlobalFilterLandingPag" sheetId="1" r:id="rId1"/>
@@ -2011,7 +2011,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2329,14 +2329,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="139.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="205.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>